<commit_message>
Fix minor bug and format output data in the order of input
</commit_message>
<xml_diff>
--- a/excelFiles/competitor2.xlsx
+++ b/excelFiles/competitor2.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -427,24 +427,28 @@
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Qwil Apartments</v>
+        <v>WILCO Apartments</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">2 bed: 3
+        <v xml:space="preserve">Studio: 1
+1 bed: 4
+2 bed: 2
 Percent: %</v>
       </c>
       <c r="C2" t="str">
-        <v>none</v>
-      </c>
-      <c r="D2" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="E2" t="str">
-        <v>n/a</v>
+        <v>Up to 3 Weeks Free! *Restrictions Apply, Contact for Details</v>
+      </c>
+      <c r="D2" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2091
+($3.46)</v>
+      </c>
+      <c r="E2" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2780-3005
+($3.36-4.18)</v>
       </c>
       <c r="F2" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $4025-4325
-($3.66-4.13)</v>
+        <v xml:space="preserve">6/2: $3299-3459
+($3.06-3.37)</v>
       </c>
       <c r="G2" t="str">
         <v>n/a</v>
@@ -452,84 +456,86 @@
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>Hallasan</v>
+        <v>The Chadwick</v>
       </c>
       <c r="B3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 11
-1 bed: 26
-2 bed: 34
-3 bed: 16
+        <v xml:space="preserve">Studio: 10
+1 bed: 5
+2 bed: 13
 Percent: %</v>
       </c>
       <c r="C3" t="str">
-        <v>Now Offering Up to 8 Weeks Rent Credit! Restrictions Apply, Contact Us Today!</v>
+        <v>none</v>
       </c>
       <c r="D3" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2385-2830
-($4.57-5.59)</v>
+        <v xml:space="preserve">6/2: $1460-1575
+($3.42-4.04)</v>
       </c>
       <c r="E3" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3570-5999
-($4.16-5.01)</v>
+        <v xml:space="preserve">6/2: $1809-1849
+($2.79-2.85)</v>
       </c>
       <c r="F3" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $4398-8284
-($3.73-5.43)</v>
-      </c>
-      <c r="G3" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $5086-9274
-($3.55-5.13)</v>
+        <v xml:space="preserve">6/2: $2634-2809
+($2.4-2.96)</v>
+      </c>
+      <c r="G3" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>4749 Elmwood Ave</v>
+        <v>The 900</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">1 bed: 1
-3 bed: 3
+        <v xml:space="preserve">Studio: 5
+1 bed: 13
+2 bed: 2
 Percent: %</v>
       </c>
       <c r="C4" t="str">
         <v>none</v>
       </c>
-      <c r="D4" t="str">
-        <v>n/a</v>
+      <c r="D4" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2200-2550
+($4-4.48)</v>
       </c>
       <c r="E4" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2599
-($3.32)</v>
-      </c>
-      <c r="F4" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="G4" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $1140-1249
-($Infinity)</v>
+        <v xml:space="preserve">6/2: $2392-3433
+($3.48-4.62)</v>
+      </c>
+      <c r="F4" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $3250-3934
+($3.87-4.16)</v>
+      </c>
+      <c r="G4" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
       <c r="A5" t="str">
-        <v>Rise Koreatown</v>
+        <v>Fedora x Trilby</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 7
-1 bed: 13
+        <v xml:space="preserve">Studio: 6
+1 bed: 3
+2 bed: 12
 Percent: %</v>
       </c>
       <c r="C5" t="str">
-        <v>Up to 6 Weeks Free + $1000 Look &amp; Lease Special! *Restrictions Apply, On Select Units</v>
+        <v>Lease Today &amp; Receive One Month Rent FREE!! This special offer is available for a limited time only.</v>
       </c>
       <c r="D5" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2360-2445
-($5.16-5.35)</v>
+        <v xml:space="preserve">6/2: $1980-2221
+($3.86-4.51)</v>
       </c>
       <c r="E5" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3320-4465
-($3.99-6.31)</v>
-      </c>
-      <c r="F5" t="str">
-        <v>n/a</v>
+        <v xml:space="preserve">6/2: $2501-2753
+($3.53-3.59)</v>
+      </c>
+      <c r="F5" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2937-3626
+($2.83-3.28)</v>
       </c>
       <c r="G5" t="str">
         <v>n/a</v>
@@ -537,25 +543,24 @@
     </row>
     <row r="6" xml:space="preserve">
       <c r="A6" t="str">
-        <v>Fedora x Trilby</v>
+        <v>Qwil Apartments</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 4
-1 bed: 4
-2 bed: 11
+        <v xml:space="preserve">2 bed: 2
 Percent: %</v>
       </c>
       <c r="C6" t="str">
-        <v>Lease Today &amp; Receive One Month Rent FREE!! This special offer is available for a limited time only.</v>
+        <v>none</v>
       </c>
       <c r="D6" t="str">
-        <v>5/20: $0-2095</v>
+        <v>n/a</v>
       </c>
       <c r="E6" t="str">
-        <v>5/20: $0-2617</v>
-      </c>
-      <c r="F6" t="str">
-        <v>5/20: $0-3570</v>
+        <v>n/a</v>
+      </c>
+      <c r="F6" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $3895-4325
+($3.53-4.13)</v>
       </c>
       <c r="G6" t="str">
         <v>n/a</v>
@@ -563,23 +568,21 @@
     </row>
     <row r="7" xml:space="preserve">
       <c r="A7" t="str">
-        <v>Miles at Harvard</v>
+        <v>The Rhys</v>
       </c>
       <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 9
-1 bed: 4
+        <v xml:space="preserve">1 bed: 1
 Percent: %</v>
       </c>
       <c r="C7" t="str">
-        <v>none</v>
-      </c>
-      <c r="D7" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $1407-2750
-($6.77-Infinity)</v>
+        <v>Leasing Special ~ 1 month free on 15 months lease! Lease today and receive free parking for one year! Contact leasing center for details.</v>
+      </c>
+      <c r="D7" t="str">
+        <v>n/a</v>
       </c>
       <c r="E7" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2009-2494
-($6.11-Infinity)</v>
+        <v xml:space="preserve">6/2: $2425
+($3.77)</v>
       </c>
       <c r="F7" t="str">
         <v>n/a</v>
@@ -590,24 +593,26 @@
     </row>
     <row r="8" xml:space="preserve">
       <c r="A8" t="str">
-        <v>The Rhys</v>
+        <v>Berkshire K2LA</v>
       </c>
       <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">2 bed: 2
+        <v xml:space="preserve">Studio: 5
+1 bed: 2
 Percent: %</v>
       </c>
       <c r="C8" t="str">
-        <v>Leasing Special ~ 1 month free on 15 months lease! Lease today and receive free parking for one year! Contact leasing center for details.</v>
-      </c>
-      <c r="D8" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="E8" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="F8" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3495-3895
-($2.91-3.24)</v>
+        <v>ASK US HOW TO GET 2 WEEKS FREE!* *Terms &amp; restrictions apply/select apartments/subject to end without notice. ASK ABOUT OUR 2 BEDROOM FEATURED FLOORPLAN!</v>
+      </c>
+      <c r="D8" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $1974-2409
+($4.18-4.7)</v>
+      </c>
+      <c r="E8" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2389-2754
+($3.73-4.1)</v>
+      </c>
+      <c r="F8" t="str">
+        <v>n/a</v>
       </c>
       <c r="G8" t="str">
         <v>n/a</v>
@@ -615,47 +620,53 @@
     </row>
     <row r="9" xml:space="preserve">
       <c r="A9" t="str">
-        <v>The BORA 3170</v>
+        <v>4749 Elmwood Ave</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">1 bed: 8
+        <v xml:space="preserve">1 bed: 1
 2 bed: 1
+3 bed: 5
+4 bed: 4
 Percent: %</v>
       </c>
       <c r="C9" t="str">
-        <v>*Up to 12 Weeks of Free Rent! *1. 13 month lease = 8 weeks free *2. 20 month lease = 12 weeks free - $50 discount on parking fee each month for the entire lease period (Original fee $100/month) *3. $200 Amazon gift card for new tenants *4. $500 credit towards the rent for look and lease (within 24 hours of the tour) **All concessions are included in the rent/price amount.</v>
+        <v>none</v>
       </c>
       <c r="D9" t="str">
         <v>n/a</v>
       </c>
       <c r="E9" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2444-3152
-($3.89-4.41)</v>
+        <v xml:space="preserve">6/2: $2599
+($3.32)</v>
       </c>
       <c r="F9" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3525
+        <v xml:space="preserve">6/2: $2900
+($5.07)</v>
+      </c>
+      <c r="G9" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $1140-3790
 ($3.6)</v>
-      </c>
-      <c r="G9" t="str">
-        <v>n/a</v>
       </c>
     </row>
     <row r="10" xml:space="preserve">
       <c r="A10" t="str">
-        <v>Park Wilshire Apartments</v>
+        <v>Rise Koreatown</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">
+        <v xml:space="preserve">Studio: 8
+1 bed: 16
 Percent: %</v>
       </c>
       <c r="C10" t="str">
-        <v>None</v>
-      </c>
-      <c r="D10" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="E10" t="str">
-        <v>n/a</v>
+        <v>Up to 6 Weeks Free + $1000 Look &amp; Lease Special! *Restrictions Apply, On Select Units</v>
+      </c>
+      <c r="D10" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2410-2530
+($5.27-5.54)</v>
+      </c>
+      <c r="E10" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2760-4550
+($3.99-6.31)</v>
       </c>
       <c r="F10" t="str">
         <v>n/a</v>
@@ -666,28 +677,28 @@
     </row>
     <row r="11" xml:space="preserve">
       <c r="A11" t="str">
-        <v>The 900</v>
+        <v>2783 Francis Ave</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 5
-1 bed: 12
-2 bed: 2
+        <v xml:space="preserve">Studio: 1
+1 bed: 2
+2 bed: 6
 Percent: %</v>
       </c>
       <c r="C11" t="str">
-        <v>none</v>
+        <v>We are offering up to 6 weeks free rent on a 13 month lease on selected units on approved credit. ** Discounts are already reflected in the price listed</v>
       </c>
       <c r="D11" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2200-2496
-($4-4.48)</v>
+        <v xml:space="preserve">6/2: $2125
+($3.42)</v>
       </c>
       <c r="E11" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2390-3433
-($3.83-4.62)</v>
+        <v xml:space="preserve">6/2: $2700-2745
+($2.74-2.78)</v>
       </c>
       <c r="F11" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3697-3934
-($3.93-4.16)</v>
+        <v xml:space="preserve">6/2: $2790-3785
+($2.76-3.17)</v>
       </c>
       <c r="G11" t="str">
         <v>n/a</v>
@@ -695,176 +706,123 @@
     </row>
     <row r="12" xml:space="preserve">
       <c r="A12" t="str">
-        <v>WILCO Apartments</v>
+        <v>Hollywood Flats</v>
       </c>
       <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
-1 bed: 3
-2 bed: 2
-Percent: %</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Up to 4 Weeks Free PLUS $750 Look &amp; Lease Special! *Select Units Only, Contact for Details</v>
-      </c>
-      <c r="D12" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2148
-($4.11)</v>
-      </c>
-      <c r="E12" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2780-2870
-($3.36-4.18)</v>
-      </c>
-      <c r="F12" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3181-3281
-($3.04-3.44)</v>
-      </c>
-      <c r="G12" t="str">
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="13" xml:space="preserve">
-      <c r="A13" t="str">
-        <v>Berkshire K2LA</v>
-      </c>
-      <c r="B13" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 5
-1 bed: 1
-2 bed: 1
-Percent: %</v>
-      </c>
-      <c r="C13" t="str">
-        <v>ASK ABOUT OUR 2 BEDROOM FEATURED FLOORPLAN!</v>
-      </c>
-      <c r="D13" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $1974-2385
-($4.34-4.7)</v>
-      </c>
-      <c r="E13" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2584
-($3.85)</v>
-      </c>
-      <c r="F13" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3161
-($3.11)</v>
-      </c>
-      <c r="G13" t="str">
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="14" xml:space="preserve">
-      <c r="A14" t="str">
-        <v>Views</v>
-      </c>
-      <c r="B14" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-Percent: %</v>
-      </c>
-      <c r="C14" t="str">
-        <v>none</v>
-      </c>
-      <c r="D14" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="E14" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="F14" t="str">
-        <v>n/a</v>
-      </c>
-      <c r="G14" t="str">
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="15" xml:space="preserve">
-      <c r="A15" t="str">
-        <v>Hollywood Flats</v>
-      </c>
-      <c r="B15" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 1
 1 bed: 13
 2 bed: 27
 Percent: %</v>
       </c>
+      <c r="C12" t="str">
+        <v>none</v>
+      </c>
+      <c r="D12" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2245
+($3.74)</v>
+      </c>
+      <c r="E12" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2625-2850
+($3-3.39)</v>
+      </c>
+      <c r="F12" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $3450-3675
+($2.64-3.3)</v>
+      </c>
+      <c r="G12" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="13" xml:space="preserve">
+      <c r="A13" t="str">
+        <v>Hallasan</v>
+      </c>
+      <c r="B13" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 10
+1 bed: 23
+2 bed: 34
+3 bed: 12
+Percent: %</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Now Offering Up to 8 Weeks Rent Credit! Restrictions Apply, Contact Us Today!</v>
+      </c>
+      <c r="D13" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2385-2830
+($4.57-5.59)</v>
+      </c>
+      <c r="E13" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $3622-5759
+($4.11-5.01)</v>
+      </c>
+      <c r="F13" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $4398-8044
+($3.73-5.27)</v>
+      </c>
+      <c r="G13" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $5236-8699
+($3.65-4.76)</v>
+      </c>
+    </row>
+    <row r="14" xml:space="preserve">
+      <c r="A14" t="str">
+        <v>The BORA 3170</v>
+      </c>
+      <c r="B14" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 2
+1 bed: 8
+2 bed: 1
+Percent: %</v>
+      </c>
+      <c r="C14" t="str">
+        <v>*Up to 12 Weeks of Free Rent! *1. 13 month lease = 8 weeks free *2. 20 month lease = 12 weeks free - $50 discount on parking fee each month for the entire lease period (Original fee $100/month) *3. $200 Amazon gift card for new tenants *4. $500 credit towards the rent for look and lease (within 24 hours of the tour) **All concessions are included in the rent amount.</v>
+      </c>
+      <c r="D14" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $1910-2150
+($4.47-4.68)</v>
+      </c>
+      <c r="E14" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $2444-3152
+($3.89-4.41)</v>
+      </c>
+      <c r="F14" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/2: $3660
+($3.74)</v>
+      </c>
+      <c r="G14" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="15" xml:space="preserve">
+      <c r="A15" t="str">
+        <v>Miles at Harvard</v>
+      </c>
+      <c r="B15" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 13
+1 bed: 4
+Percent: %</v>
+      </c>
       <c r="C15" t="str">
         <v>none</v>
       </c>
       <c r="D15" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2245
-($3.74)</v>
+        <v xml:space="preserve">6/2: $1407-2750
+($7.07-10.94)</v>
       </c>
       <c r="E15" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2625-2850
-($3-3.39)</v>
-      </c>
-      <c r="F15" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $3450-3675
-($2.64-3.3)</v>
+        <v xml:space="preserve">6/2: $2009-2494
+($6.11)</v>
+      </c>
+      <c r="F15" t="str">
+        <v>n/a</v>
       </c>
       <c r="G15" t="str">
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="16" xml:space="preserve">
-      <c r="A16" t="str">
-        <v>The Chadwick</v>
-      </c>
-      <c r="B16" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 10
-1 bed: 5
-2 bed: 14
-Percent: %</v>
-      </c>
-      <c r="C16" t="str">
-        <v>none</v>
-      </c>
-      <c r="D16" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $1447-1627
-($3.45-3.91)</v>
-      </c>
-      <c r="E16" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $1809-1874
-($2.79-2.89)</v>
-      </c>
-      <c r="F16" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2520-2710
-($2.37-2.85)</v>
-      </c>
-      <c r="G16" t="str">
-        <v>n/a</v>
-      </c>
-    </row>
-    <row r="17" xml:space="preserve">
-      <c r="A17" t="str">
-        <v>2783 Francis Ave</v>
-      </c>
-      <c r="B17" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
-1 bed: 2
-2 bed: 6
-Percent: %</v>
-      </c>
-      <c r="C17" t="str">
-        <v>We are offering up to 6 weeks free rent on a 13 month lease on selected units on approved credit. ** Discounts are already reflected in the price listed</v>
-      </c>
-      <c r="D17" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2125
-($3.42)</v>
-      </c>
-      <c r="E17" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2700-2745
-($2.74-2.78)</v>
-      </c>
-      <c r="F17" t="str" xml:space="preserve">
-        <v xml:space="preserve">5/20: $2790-3785
-($2.76-3.17)</v>
-      </c>
-      <c r="G17" t="str">
         <v>n/a</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>